<commit_message>
5 more super-adventure img
</commit_message>
<xml_diff>
--- a/super-adventure-game/checklist.xlsx
+++ b/super-adventure-game/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/super-adventure-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF8F635C-FB33-4949-9DE6-79DE8D9FDF19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889ABD54-4FA6-6F4F-8BB8-E136826E01D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{01552798-BB71-8343-BFB6-09AF7D3B2DDC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
   <si>
     <t>year</t>
   </si>
@@ -312,6 +312,60 @@
   </si>
   <si>
     <t>wolfhead_strikes_back.jpg</t>
+  </si>
+  <si>
+    <t>吸血鬼の洞窟</t>
+  </si>
+  <si>
+    <t>vampire_cave.jpg</t>
+  </si>
+  <si>
+    <t>シャドー砦の魔王</t>
+  </si>
+  <si>
+    <t>demon_king_of_fort_shadow.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">炎の神殿 </t>
+  </si>
+  <si>
+    <t>Crypt of the Vampire</t>
+  </si>
+  <si>
+    <t>The Lord of Shadow Keep</t>
+  </si>
+  <si>
+    <t>The Temple of Flame</t>
+  </si>
+  <si>
+    <t>失われた魂の城</t>
+  </si>
+  <si>
+    <t>Castle of Lost Souls</t>
+  </si>
+  <si>
+    <t>castle_of_lost_souls.jpg</t>
+  </si>
+  <si>
+    <t>temple_of_the_flame.jpg</t>
+  </si>
+  <si>
+    <t>ドラゴンの目</t>
+  </si>
+  <si>
+    <t>The Eye of the Dragon</t>
+  </si>
+  <si>
+    <t>eye_of_the_dragon.jpg</t>
+  </si>
+  <si>
+    <t>ファラオの呪い</t>
+  </si>
+  <si>
+    <t>Curse of the Pharaoh</t>
+  </si>
+  <si>
+    <t>curse_of_the_pharaoh.jpg</t>
   </si>
 </sst>
 </file>
@@ -672,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE28C76-E3E7-7B41-A0B5-06A554F52F34}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,6 +1250,108 @@
         <v>92</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1986</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1986</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1986</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1986</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1986</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1986</v>
+      </c>
+      <c r="B36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>